<commit_message>
Login y registro terminado
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/menus.xlsx
+++ b/src/main/resources/Data/menus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nintech\Proyectos\Programas\java\WherEat\WherEat\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B92734-408D-434B-8AD8-66BD4F34DB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E70DA-491B-44B6-B5C1-C73A4C843741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="262">
   <si>
     <t>Biblioteca central</t>
   </si>
@@ -806,6 +806,30 @@
   </si>
   <si>
     <t>A134340</t>
+  </si>
+  <si>
+    <t>Fabian</t>
+  </si>
+  <si>
+    <t>Guia</t>
+  </si>
+  <si>
+    <t>prueba@gmail.com</t>
+  </si>
+  <si>
+    <t>Aram</t>
+  </si>
+  <si>
+    <t>Gonzales</t>
+  </si>
+  <si>
+    <t>correogenerico@gmail.com</t>
+  </si>
+  <si>
+    <t>algo1234</t>
+  </si>
+  <si>
+    <t>contraseña</t>
   </si>
 </sst>
 </file>
@@ -937,8 +961,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34FE7A4C-4AF9-42B2-B81A-40279E759F80}" name="Tabla1" displayName="Tabla1" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{34FE7A4C-4AF9-42B2-B81A-40279E759F80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34FE7A4C-4AF9-42B2-B81A-40279E759F80}" name="Tabla1" displayName="Tabla1" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{34FE7A4C-4AF9-42B2-B81A-40279E759F80}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{04D57AF8-9FFB-4E94-AF07-AFAC6C77B6D3}" name="Nombres"/>
     <tableColumn id="2" xr3:uid="{716EEDB6-DE4B-45B8-8104-3D089AF9A671}" name="Apellidos"/>
@@ -1337,7 +1361,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,9 +1401,32 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
+      <c r="A3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>260</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4060,6 +4107,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005468605E04F61747936F12076C15E824" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ad5602634390927fddd3c2a70f7b49c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d86c30-c586-4855-827a-97f18e7b00d3" xmlns:ns4="db3c7e19-2d34-4eb7-903f-b25b7c5160ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efd1d29f83cac9fbca6e4254de116c19" ns3:_="" ns4:_="">
     <xsd:import namespace="77d86c30-c586-4855-827a-97f18e7b00d3"/>
@@ -4288,38 +4352,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
-    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4342,9 +4378,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
+    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
solo falta mostrar y poder navegar en los datos
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/menus.xlsx
+++ b/src/main/resources/Data/menus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nintech\Proyectos\Programas\java\WherEat\WherEat\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E70DA-491B-44B6-B5C1-C73A4C843741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC4701D-E677-44AA-9703-3F3517414F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="8" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="5" r:id="rId1"/>
@@ -44,10 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="262">
-  <si>
-    <t>Biblioteca central</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="272">
   <si>
     <t>Precio</t>
   </si>
@@ -830,13 +827,46 @@
   </si>
   <si>
     <t>contraseña</t>
+  </si>
+  <si>
+    <t>Cafeteria</t>
+  </si>
+  <si>
+    <t>7:30 am - 5:00 pm</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Turismo</t>
+  </si>
+  <si>
+    <t>Arquitectura</t>
+  </si>
+  <si>
+    <t>Geografia</t>
+  </si>
+  <si>
+    <t>Ingenieria</t>
+  </si>
+  <si>
+    <t>Biblioteca Central</t>
+  </si>
+  <si>
+    <t>Biblioteca_Central</t>
+  </si>
+  <si>
+    <t>Humanidades</t>
+  </si>
+  <si>
+    <t>Contaduria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +892,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -974,88 +1010,120 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}" name="Tabla6" displayName="Tabla6" ref="A1:B46" totalsRowShown="0">
-  <autoFilter ref="A1:B46" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}" name="Tabla6" displayName="Tabla6" ref="A1:F46" totalsRowShown="0">
+  <autoFilter ref="A1:F46" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1AAD8D7D-8ACC-4B9D-8E5A-D9DB57E67781}" name="Facultad de turismo"/>
     <tableColumn id="2" xr3:uid="{1BF85A86-FC1D-4096-A9C4-7B92A4927378}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{ADA2A64D-2FE4-428A-A832-11E5B9B5A25D}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{81685046-EB44-468C-AFB0-FD365FBA0639}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{9F4D72F1-E655-49B0-A814-51CCB7E233B1}" name="10"/>
+    <tableColumn id="6" xr3:uid="{F6F940CB-0524-4A14-96D1-9F695908AF44}" name="Turismo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6249AEDA-77C5-4418-A311-5EE08F815252}" name="Tabla5" displayName="Tabla5" ref="A1:B25" totalsRowShown="0">
-  <autoFilter ref="A1:B25" xr:uid="{6249AEDA-77C5-4418-A311-5EE08F815252}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6249AEDA-77C5-4418-A311-5EE08F815252}" name="Tabla5" displayName="Tabla5" ref="A1:F25" totalsRowShown="0">
+  <autoFilter ref="A1:F25" xr:uid="{6249AEDA-77C5-4418-A311-5EE08F815252}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B49ABD42-428B-49CE-BE09-E4A11739540C}" name="Facultad de arquitectura "/>
     <tableColumn id="2" xr3:uid="{D65570A7-804B-4D1C-A64E-6FC8C633E8B2}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{B8F449BE-986E-4AAE-B194-F5951B77DC97}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{D3AFE0D3-1960-43A4-AA99-C1C062FDADB8}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{8AF0D127-53EE-4FCB-8CA3-B879770A12F8}" name="10"/>
+    <tableColumn id="6" xr3:uid="{EE65DE86-E1B2-43E5-AD8D-14625572B957}" name="Arquitectura"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07BFC840-08DF-4785-A852-7B557697E0EE}" name="Tabla4" displayName="Tabla4" ref="A1:B24" totalsRowShown="0">
-  <autoFilter ref="A1:B24" xr:uid="{07BFC840-08DF-4785-A852-7B557697E0EE}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{07BFC840-08DF-4785-A852-7B557697E0EE}" name="Tabla4" displayName="Tabla4" ref="A1:F24" totalsRowShown="0">
+  <autoFilter ref="A1:F24" xr:uid="{07BFC840-08DF-4785-A852-7B557697E0EE}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3919A4F0-ECA4-4CCD-A1B6-B52224F63208}" name="Facultad de geografia"/>
     <tableColumn id="2" xr3:uid="{51569CC2-13F1-4AF3-860E-9F0F54A2CEDC}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{C36C4E2C-69E7-4D8A-B44D-947B599747A8}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{5EB201DD-A2BC-42CA-8196-12BBAE11C0E2}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{CDD3D419-F2C6-4AAE-8EEB-8B20E9954C77}" name="10"/>
+    <tableColumn id="6" xr3:uid="{B380BF19-D676-4E02-9B74-D3CC5B40783B}" name="Geografia"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13E0910E-B03F-4612-8FAD-EFA73B225EE9}" name="Tabla3" displayName="Tabla3" ref="A1:B42" totalsRowShown="0">
-  <autoFilter ref="A1:B42" xr:uid="{13E0910E-B03F-4612-8FAD-EFA73B225EE9}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{13E0910E-B03F-4612-8FAD-EFA73B225EE9}" name="Tabla3" displayName="Tabla3" ref="A1:F42" totalsRowShown="0">
+  <autoFilter ref="A1:F42" xr:uid="{13E0910E-B03F-4612-8FAD-EFA73B225EE9}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{118A8A06-5ED6-482E-9942-80DA257CF408}" name="Facultad de ingenieria "/>
     <tableColumn id="2" xr3:uid="{F0606ED8-3B88-41DD-954A-A91E5865CEE5}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{F692AAE7-02D7-421A-BDC5-99AD841125C2}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{76335891-3A80-4847-8EDB-F81EF1E1A1EC}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{14F9AC61-AB56-4CC3-BE10-242864208BB8}" name="10"/>
+    <tableColumn id="6" xr3:uid="{7A8F2A5A-7C75-44DD-BEB5-AD76D043895D}" name="Ingenieria"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{258CD1A2-74B2-418B-A9CE-68A2E2EB8FB2}" name="Tabla2" displayName="Tabla2" ref="A1:B42" totalsRowShown="0">
-  <autoFilter ref="A1:B42" xr:uid="{258CD1A2-74B2-418B-A9CE-68A2E2EB8FB2}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8E2F33C8-5794-4F0A-80A6-E7BF3397686B}" name="Biblioteca central"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{258CD1A2-74B2-418B-A9CE-68A2E2EB8FB2}" name="Tabla2" displayName="Tabla2" ref="A1:F42" totalsRowShown="0">
+  <autoFilter ref="A1:F42" xr:uid="{258CD1A2-74B2-418B-A9CE-68A2E2EB8FB2}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8E2F33C8-5794-4F0A-80A6-E7BF3397686B}" name="Biblioteca_Central"/>
     <tableColumn id="2" xr3:uid="{29117603-85D9-4527-82CA-B1EB0DC5B2E3}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{FBC563C8-0C58-48B0-B4BB-88A9E5C27C86}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{DFD10B22-75D7-4CA4-8BB1-774942A9F4E8}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{A46AFDE4-0113-4BE2-99F0-AD86F400CB41}" name="10"/>
+    <tableColumn id="6" xr3:uid="{AB8AB8EB-35BE-44E4-9EBE-AF509E3151A1}" name="Biblioteca Central"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04550AF8-6959-44A8-8A74-5A1C67CE5A8B}" name="Tabla9" displayName="Tabla9" ref="A1:B24" totalsRowShown="0">
-  <autoFilter ref="A1:B24" xr:uid="{04550AF8-6959-44A8-8A74-5A1C67CE5A8B}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04550AF8-6959-44A8-8A74-5A1C67CE5A8B}" name="Tabla9" displayName="Tabla9" ref="A1:F24" totalsRowShown="0">
+  <autoFilter ref="A1:F24" xr:uid="{04550AF8-6959-44A8-8A74-5A1C67CE5A8B}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C9B27706-6060-476F-96A5-3E43CB8A5FF4}" name="Facultad de humanidades"/>
     <tableColumn id="2" xr3:uid="{E417E1EE-FD4E-4BC8-8DAE-6C7370BF05A6}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{B431B207-19C5-4FB4-87E6-AE48C2FCA1E5}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{FDD2C804-C462-4C69-94BE-FF5A158907FB}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{4C10C281-3B2F-45EB-A6E9-CD8761C06751}" name="10"/>
+    <tableColumn id="6" xr3:uid="{B5491032-6804-48FB-8BCF-8C4BE59DC784}" name="Humanidades"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}" name="Tabla8" displayName="Tabla8" ref="A1:B40" totalsRowShown="0">
-  <autoFilter ref="A1:B40" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}" name="Tabla8" displayName="Tabla8" ref="A1:F40" totalsRowShown="0">
+  <autoFilter ref="A1:F40" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9C0B3A76-B193-4AE7-91AF-646A8F39B4BA}" name="Facultad de contaduria" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{319EA91E-DEB4-4A8C-B6CA-D5E3ACDE8BF5}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{118181F1-C7EB-424B-A3FC-F13F4107D3A0}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{E048953C-E521-4C46-9283-FFAC59C613F0}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{897E1CA2-0BE0-4685-91D2-D07C22AFF44D}" name="10"/>
+    <tableColumn id="6" xr3:uid="{9D8A5C6D-468E-419D-8DF0-EDC1785C2DC3}" name="Contaduria"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}" name="Tabla7" displayName="Tabla7" ref="A1:B69" totalsRowShown="0">
-  <autoFilter ref="A1:B69" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}" name="Tabla7" displayName="Tabla7" ref="A1:F69" totalsRowShown="0">
+  <autoFilter ref="A1:F69" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CDEE3D85-FBD8-482C-8A46-E15B63C03A45}" name="Facultad de economia " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{FFAD0A33-DFAD-4A2C-A02B-338DE51DE232}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{6251E98E-4A98-471E-97DC-E18B88173762}" name="Cafeteria"/>
+    <tableColumn id="4" xr3:uid="{D7CDE4AE-E3D7-47BE-8C10-AC61BC653E53}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{2A8D577E-FE44-44E9-836C-0E1646DD8923}" name="10"/>
+    <tableColumn id="6" xr3:uid="{EB26EF0C-5CC5-489B-8AAF-91F6067CC3C2}" name="Contaduria"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1360,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECF5DA-6B46-4C56-8004-333EE01336D6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,58 +1442,58 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
         <v>246</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>247</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>252</v>
-      </c>
-      <c r="D2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
         <v>254</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B4" t="s">
         <v>257</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>258</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>259</v>
-      </c>
-      <c r="D4" t="s">
-        <v>260</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -1437,148 +1505,165 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F099B287-23BF-45F2-A67E-A80C884E73AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073E5BC-8B24-4A79-8D19-767842E46DB6}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>119</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>120</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <v>30</v>
@@ -1586,7 +1671,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17">
         <v>22</v>
@@ -1594,7 +1679,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18">
         <v>30</v>
@@ -1602,7 +1687,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19">
         <v>35</v>
@@ -1610,7 +1695,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -1618,7 +1703,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21">
         <v>29</v>
@@ -1626,7 +1711,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22">
         <v>25</v>
@@ -1634,7 +1719,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23">
         <v>30</v>
@@ -1642,7 +1727,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24">
         <v>27</v>
@@ -1650,7 +1735,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25">
         <v>27</v>
@@ -1658,7 +1743,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26">
         <v>55</v>
@@ -1666,7 +1751,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>35</v>
@@ -1674,7 +1759,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28">
         <v>25</v>
@@ -1682,7 +1767,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -1690,7 +1775,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30">
         <v>25</v>
@@ -1698,7 +1783,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -1706,7 +1791,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B32">
         <v>50</v>
@@ -1714,7 +1799,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33">
         <v>35</v>
@@ -1722,7 +1807,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>35</v>
@@ -1730,7 +1815,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B35">
         <v>35</v>
@@ -1738,7 +1823,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36">
         <v>20</v>
@@ -1746,7 +1831,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>40</v>
@@ -1754,7 +1839,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B38">
         <v>40</v>
@@ -1762,7 +1847,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39">
         <v>40</v>
@@ -1770,7 +1855,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40">
         <v>55</v>
@@ -1778,7 +1863,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41">
         <v>70</v>
@@ -1786,7 +1871,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -1794,7 +1879,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43">
         <v>40</v>
@@ -1802,7 +1887,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44">
         <v>48</v>
@@ -1810,7 +1895,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45">
         <v>70</v>
@@ -1818,13 +1903,14 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1834,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8C8FDA-A599-404E-95E0-74FEAB4F17F7}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,129 +1931,141 @@
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>94</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16">
         <v>200</v>
@@ -1975,7 +2073,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>60</v>
@@ -1983,7 +2081,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -1991,7 +2089,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -1999,7 +2097,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20">
         <v>16</v>
@@ -2007,7 +2105,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21">
         <v>25</v>
@@ -2015,7 +2113,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22">
         <v>30</v>
@@ -2023,7 +2121,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23">
         <v>30</v>
@@ -2031,7 +2129,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -2039,13 +2137,14 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25">
         <v>35</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2055,138 +2154,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0067CAE2-AC93-4F63-870E-8F25CB971E28}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -2194,7 +2307,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17">
         <v>65</v>
@@ -2202,7 +2315,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18">
         <v>60</v>
@@ -2210,7 +2323,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -2218,7 +2331,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20">
         <v>45</v>
@@ -2226,7 +2339,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21">
         <v>35</v>
@@ -2234,7 +2347,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>50</v>
@@ -2242,7 +2355,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>15</v>
@@ -2250,13 +2363,14 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>65</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2266,140 +2380,153 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048A8DEB-3D6C-404C-97ED-45E942345101}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <v>50</v>
@@ -2407,7 +2534,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <v>60</v>
@@ -2415,7 +2542,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -2423,7 +2550,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -2431,7 +2558,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>40</v>
@@ -2439,7 +2566,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>40</v>
@@ -2447,7 +2574,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>60</v>
@@ -2455,7 +2582,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>25</v>
@@ -2463,7 +2590,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>30</v>
@@ -2471,7 +2598,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>30</v>
@@ -2479,7 +2606,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2487,7 +2614,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -2495,7 +2622,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>50</v>
@@ -2503,7 +2630,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -2511,7 +2638,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30">
         <v>60</v>
@@ -2519,7 +2646,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -2527,7 +2654,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>50</v>
@@ -2535,7 +2662,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>40</v>
@@ -2543,7 +2670,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34">
         <v>60</v>
@@ -2551,7 +2678,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>55</v>
@@ -2559,7 +2686,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36">
         <v>65</v>
@@ -2567,7 +2694,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>45</v>
@@ -2575,7 +2702,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>50</v>
@@ -2583,7 +2710,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>100</v>
@@ -2591,7 +2718,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>80</v>
@@ -2599,7 +2726,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>70</v>
@@ -2607,13 +2734,14 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2623,140 +2751,153 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379224EA-4FD9-4D93-913B-ACD011DCBC75}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>55</v>
@@ -2764,7 +2905,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>55</v>
@@ -2772,7 +2913,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -2780,7 +2921,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -2788,7 +2929,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -2796,7 +2937,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>45</v>
@@ -2804,7 +2945,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>30</v>
@@ -2812,7 +2953,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>30</v>
@@ -2820,7 +2961,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>30</v>
@@ -2828,7 +2969,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>33</v>
@@ -2836,7 +2977,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>33</v>
@@ -2844,7 +2985,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -2852,7 +2993,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>45</v>
@@ -2860,7 +3001,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>45</v>
@@ -2868,7 +3009,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -2876,7 +3017,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>45</v>
@@ -2884,7 +3025,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>40</v>
@@ -2892,7 +3033,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>40</v>
@@ -2900,7 +3041,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>43</v>
@@ -2908,7 +3049,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>55</v>
@@ -2916,7 +3057,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>55</v>
@@ -2924,7 +3065,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>43</v>
@@ -2932,7 +3073,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>55</v>
@@ -2940,7 +3081,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>55</v>
@@ -2948,7 +3089,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>45</v>
@@ -2956,7 +3097,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>55</v>
@@ -2964,13 +3105,14 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2980,140 +3122,153 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100AFF4A-8751-43FB-87B9-A3011D49E575}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B9">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B14">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16">
         <v>60</v>
@@ -3121,7 +3276,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -3129,7 +3284,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -3137,7 +3292,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -3145,7 +3300,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -3153,7 +3308,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21">
         <v>35</v>
@@ -3161,7 +3316,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22">
         <v>35</v>
@@ -3169,7 +3324,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23">
         <v>50</v>
@@ -3177,13 +3332,14 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3193,140 +3349,153 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2ABE09-AD8E-46CE-A995-16FFB0F48E9B}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B8">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16">
         <v>40</v>
@@ -3334,7 +3503,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17">
         <v>40</v>
@@ -3342,7 +3511,7 @@
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18">
         <v>55</v>
@@ -3350,7 +3519,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -3358,7 +3527,7 @@
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -3366,7 +3535,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>30</v>
@@ -3374,7 +3543,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22">
         <v>30</v>
@@ -3382,7 +3551,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23">
         <v>35</v>
@@ -3390,7 +3559,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>35</v>
@@ -3398,7 +3567,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25">
         <v>55</v>
@@ -3406,7 +3575,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B26">
         <v>35</v>
@@ -3414,7 +3583,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B27">
         <v>35</v>
@@ -3422,7 +3591,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28">
         <v>40</v>
@@ -3430,7 +3599,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B29">
         <v>40</v>
@@ -3438,7 +3607,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -3446,7 +3615,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31">
         <v>45</v>
@@ -3454,7 +3623,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>18</v>
@@ -3462,7 +3631,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B33">
         <v>22</v>
@@ -3470,7 +3639,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34">
         <v>22</v>
@@ -3478,7 +3647,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B35">
         <v>30</v>
@@ -3486,7 +3655,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B36">
         <v>28</v>
@@ -3494,7 +3663,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B37">
         <v>30</v>
@@ -3502,7 +3671,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38">
         <v>30</v>
@@ -3510,7 +3679,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B39">
         <v>25</v>
@@ -3518,13 +3687,14 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B40">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -3535,140 +3705,153 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5CF38E-1757-4D28-AE1C-6EFE4AED49B6}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16">
         <v>50</v>
@@ -3676,7 +3859,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B17">
         <v>60</v>
@@ -3684,7 +3867,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -3692,7 +3875,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -3700,7 +3883,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>40</v>
@@ -3708,7 +3891,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>40</v>
@@ -3716,7 +3899,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>60</v>
@@ -3724,7 +3907,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>25</v>
@@ -3732,7 +3915,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>30</v>
@@ -3740,7 +3923,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>37</v>
@@ -3748,7 +3931,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>29</v>
@@ -3756,7 +3939,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -3764,7 +3947,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>50</v>
@@ -3772,7 +3955,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -3780,7 +3963,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B30">
         <v>55</v>
@@ -3788,7 +3971,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B31">
         <v>55</v>
@@ -3796,7 +3979,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B32">
         <v>55</v>
@@ -3804,7 +3987,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B33">
         <v>55</v>
@@ -3812,7 +3995,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B34">
         <v>55</v>
@@ -3820,7 +4003,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B35">
         <v>55</v>
@@ -3828,7 +4011,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36">
         <v>62</v>
@@ -3836,7 +4019,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B37">
         <v>62</v>
@@ -3844,7 +4027,7 @@
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38">
         <v>62</v>
@@ -3852,7 +4035,7 @@
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39">
         <v>62</v>
@@ -3860,7 +4043,7 @@
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B40">
         <v>62</v>
@@ -3868,7 +4051,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B41">
         <v>62</v>
@@ -3876,7 +4059,7 @@
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42">
         <v>62</v>
@@ -3884,7 +4067,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -3892,7 +4075,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B44">
         <v>52</v>
@@ -3900,7 +4083,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B45">
         <v>46</v>
@@ -3908,7 +4091,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B46">
         <v>46</v>
@@ -3916,7 +4099,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B47">
         <v>56</v>
@@ -3924,7 +4107,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B48">
         <v>56</v>
@@ -3932,7 +4115,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B49">
         <v>56</v>
@@ -3940,7 +4123,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B50">
         <v>55</v>
@@ -3948,7 +4131,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B51">
         <v>55</v>
@@ -3956,7 +4139,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B52">
         <v>55</v>
@@ -3964,7 +4147,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53">
         <v>55</v>
@@ -3972,7 +4155,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B54">
         <v>55</v>
@@ -3980,7 +4163,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B55">
         <v>55</v>
@@ -3988,7 +4171,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B56">
         <v>62</v>
@@ -3996,7 +4179,7 @@
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B57">
         <v>62</v>
@@ -4004,7 +4187,7 @@
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B58">
         <v>62</v>
@@ -4012,7 +4195,7 @@
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B59">
         <v>62</v>
@@ -4020,7 +4203,7 @@
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B60">
         <v>62</v>
@@ -4028,7 +4211,7 @@
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B61">
         <v>62</v>
@@ -4036,7 +4219,7 @@
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B62">
         <v>62</v>
@@ -4044,7 +4227,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63">
         <v>42</v>
@@ -4052,7 +4235,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B64">
         <v>52</v>
@@ -4060,7 +4243,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B65">
         <v>46</v>
@@ -4068,7 +4251,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B66">
         <v>46</v>
@@ -4076,7 +4259,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B67">
         <v>56</v>
@@ -4084,7 +4267,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B68">
         <v>56</v>
@@ -4092,13 +4275,14 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B69">
         <v>56</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4107,23 +4291,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005468605E04F61747936F12076C15E824" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ad5602634390927fddd3c2a70f7b49c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d86c30-c586-4855-827a-97f18e7b00d3" xmlns:ns4="db3c7e19-2d34-4eb7-903f-b25b7c5160ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efd1d29f83cac9fbca6e4254de116c19" ns3:_="" ns4:_="">
     <xsd:import namespace="77d86c30-c586-4855-827a-97f18e7b00d3"/>
@@ -4352,10 +4519,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
+    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4378,20 +4573,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
-    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ya todo funciona, solo falta arreglar el registro
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/menus.xlsx
+++ b/src/main/resources/Data/menus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nintech\Proyectos\Programas\java\WherEat\WherEat\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC4701D-E677-44AA-9703-3F3517414F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3538C9C-FA07-4A4C-AF18-3F63D2FD8BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="8" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
+    <workbookView xWindow="-20460" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="5" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Humanidades" sheetId="2" r:id="rId7"/>
     <sheet name="Contaduria" sheetId="3" r:id="rId8"/>
     <sheet name="Economia" sheetId="4" r:id="rId9"/>
+    <sheet name="Cafe EDG" sheetId="11" r:id="rId10"/>
+    <sheet name="Cafe Arqui" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="287">
   <si>
     <t>Precio</t>
   </si>
@@ -496,9 +498,6 @@
     <t>Comida corrida</t>
   </si>
   <si>
-    <t xml:space="preserve">Enchiladas </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chilaquiles con huevo </t>
   </si>
   <si>
@@ -860,13 +859,61 @@
   </si>
   <si>
     <t>Contaduria</t>
+  </si>
+  <si>
+    <t>Economia</t>
+  </si>
+  <si>
+    <t>Juan Carlos</t>
+  </si>
+  <si>
+    <t>Bodoque</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facultad de Ingenieria Edificio G </t>
+  </si>
+  <si>
+    <t>Puesto de Comida</t>
+  </si>
+  <si>
+    <t>Café</t>
+  </si>
+  <si>
+    <t>Enchiladas</t>
+  </si>
+  <si>
+    <t>Café Cappuchino Largo</t>
+  </si>
+  <si>
+    <t>Café Cappuchino Corto</t>
+  </si>
+  <si>
+    <t>Chapata Italiana</t>
+  </si>
+  <si>
+    <t>Chapata Tropical</t>
+  </si>
+  <si>
+    <t>Facultad de Arquitectura - Café</t>
+  </si>
+  <si>
+    <t>Alguna</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>persona@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -902,8 +949,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,8 +971,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -925,12 +986,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -939,12 +1035,97 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1009,9 +1190,39 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1E26F61F-AFB2-461B-AFD0-CDEDA784148F}" name="Tabla11" displayName="Tabla11" ref="A1:F5" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+  <autoFilter ref="A1:F5" xr:uid="{1E26F61F-AFB2-461B-AFD0-CDEDA784148F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2E0AC016-58B3-4871-9906-B5E49973F6BF}" name="Facultad de Ingenieria Edificio G "/>
+    <tableColumn id="2" xr3:uid="{092507F2-DF02-46D8-A2B3-8B26005D584A}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{9D58D232-B48C-4E9D-8B8C-563581C1A0F4}" name="Puesto de Comida"/>
+    <tableColumn id="4" xr3:uid="{F731803E-5F32-47D9-AC94-1F6614FCF4B5}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{2B4B2B5B-F809-4CD8-8D6F-84ED72A382BD}" name="Café"/>
+    <tableColumn id="6" xr3:uid="{D2306ACD-93C6-4341-A89A-1A019FA3C02A}" name="Ingenieria"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9EB68877-7C7B-41EA-A471-B71D99C0E0A4}" name="Tabla1113" displayName="Tabla1113" ref="A1:F5" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A1:F5" xr:uid="{9EB68877-7C7B-41EA-A471-B71D99C0E0A4}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6ED70689-B90E-4FD5-950C-3302B8D3CD4D}" name="Facultad de Arquitectura - Café"/>
+    <tableColumn id="2" xr3:uid="{7ED816EE-F8AB-4DD1-80FB-F096B5BC4E84}" name="Precio"/>
+    <tableColumn id="3" xr3:uid="{5DF69C42-8797-4A96-B920-BB77729F683C}" name="Puesto de Comida"/>
+    <tableColumn id="4" xr3:uid="{55C4FB02-0529-4F86-9C66-4DD0064CCE8A}" name="7:30 am - 5:00 pm"/>
+    <tableColumn id="5" xr3:uid="{312A835D-B8B9-4632-9FC1-E6A50ECF36B5}" name="Café"/>
+    <tableColumn id="6" xr3:uid="{29C31DFD-7A75-4855-A1AA-F1001F14E3AE}" name="Arquitectura"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}" name="Tabla6" displayName="Tabla6" ref="A1:F46" totalsRowShown="0">
-  <autoFilter ref="A1:F46" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}" name="Tabla6" displayName="Tabla6" ref="A1:F47" totalsRowShown="0">
+  <autoFilter ref="A1:F47" xr:uid="{6B9768B5-0BC9-4A34-B843-8D8B7DC86173}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1AAD8D7D-8ACC-4B9D-8E5A-D9DB57E67781}" name="Facultad de turismo"/>
     <tableColumn id="2" xr3:uid="{1BF85A86-FC1D-4096-A9C4-7B92A4927378}" name="Precio"/>
@@ -1103,7 +1314,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}" name="Tabla8" displayName="Tabla8" ref="A1:F40" totalsRowShown="0">
   <autoFilter ref="A1:F40" xr:uid="{EDD1729E-E125-4AF1-BE26-74CEF6B7DB8A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9C0B3A76-B193-4AE7-91AF-646A8F39B4BA}" name="Facultad de contaduria" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9C0B3A76-B193-4AE7-91AF-646A8F39B4BA}" name="Facultad de contaduria" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{319EA91E-DEB4-4A8C-B6CA-D5E3ACDE8BF5}" name="Precio"/>
     <tableColumn id="3" xr3:uid="{118181F1-C7EB-424B-A3FC-F13F4107D3A0}" name="Cafeteria"/>
     <tableColumn id="4" xr3:uid="{E048953C-E521-4C46-9283-FFAC59C613F0}" name="7:30 am - 5:00 pm"/>
@@ -1118,12 +1329,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}" name="Tabla7" displayName="Tabla7" ref="A1:F69" totalsRowShown="0">
   <autoFilter ref="A1:F69" xr:uid="{139E0E8E-EA54-41BD-9BBA-E9ADC1B67E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CDEE3D85-FBD8-482C-8A46-E15B63C03A45}" name="Facultad de economia " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CDEE3D85-FBD8-482C-8A46-E15B63C03A45}" name="Facultad de economia " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FFAD0A33-DFAD-4A2C-A02B-338DE51DE232}" name="Precio"/>
     <tableColumn id="3" xr3:uid="{6251E98E-4A98-471E-97DC-E18B88173762}" name="Cafeteria"/>
     <tableColumn id="4" xr3:uid="{D7CDE4AE-E3D7-47BE-8C10-AC61BC653E53}" name="7:30 am - 5:00 pm"/>
     <tableColumn id="5" xr3:uid="{2A8D577E-FE44-44E9-836C-0E1646DD8923}" name="10"/>
-    <tableColumn id="6" xr3:uid="{EB26EF0C-5CC5-489B-8AAF-91F6067CC3C2}" name="Contaduria"/>
+    <tableColumn id="6" xr3:uid="{EB26EF0C-5CC5-489B-8AAF-91F6067CC3C2}" name="Economia"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1428,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECF5DA-6B46-4C56-8004-333EE01336D6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,60 +1653,88 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" t="s">
         <v>245</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>246</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
         <v>249</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>251</v>
-      </c>
-      <c r="D2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
         <v>253</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" t="s">
         <v>256</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>257</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>258</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" t="s">
         <v>259</v>
       </c>
-      <c r="E4" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
@@ -1512,12 +1751,159 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED6DD56-68DD-44C4-8648-DE7E2E79B4A7}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212F576F-77E5-4241-80DE-41BA2C1529E4}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2073E5BC-8B24-4A79-8D19-767842E46DB6}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,16 +1923,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>263</v>
-      </c>
-      <c r="F1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1871,7 +2257,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>278</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -1887,7 +2273,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44">
         <v>48</v>
@@ -1895,7 +2281,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45">
         <v>70</v>
@@ -1903,7 +2289,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -1939,16 +2325,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,7 +2543,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A25" sqref="A25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,16 +2559,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2383,7 +2769,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A43" sqref="A43:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,16 +2786,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2753,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379224EA-4FD9-4D93-913B-ACD011DCBC75}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,22 +3151,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3124,8 +3510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100AFF4A-8751-43FB-87B9-A3011D49E575}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,27 +3522,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -3164,7 +3550,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>45</v>
@@ -3172,7 +3558,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4">
         <v>57</v>
@@ -3204,7 +3590,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8">
         <v>28</v>
@@ -3212,7 +3598,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -3220,7 +3606,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -3236,7 +3622,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -3244,7 +3630,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13">
         <v>48</v>
@@ -3252,7 +3638,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -3260,7 +3646,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15">
         <v>60</v>
@@ -3276,7 +3662,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -3284,7 +3670,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -3308,7 +3694,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21">
         <v>35</v>
@@ -3316,7 +3702,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22">
         <v>35</v>
@@ -3324,7 +3710,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B23">
         <v>50</v>
@@ -3352,7 +3738,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A41" sqref="A41:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,27 +3749,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
-        <v>263</v>
-      </c>
       <c r="F1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -3391,7 +3777,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3">
         <v>45</v>
@@ -3399,7 +3785,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4">
         <v>57</v>
@@ -3407,7 +3793,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5">
         <v>36</v>
@@ -3423,7 +3809,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -3431,7 +3817,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>28</v>
@@ -3447,7 +3833,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -3455,7 +3841,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11">
         <v>30</v>
@@ -3463,7 +3849,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -3479,7 +3865,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14">
         <v>55</v>
@@ -3487,7 +3873,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15">
         <v>40</v>
@@ -3495,7 +3881,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16">
         <v>40</v>
@@ -3503,7 +3889,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17">
         <v>40</v>
@@ -3511,7 +3897,7 @@
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18">
         <v>55</v>
@@ -3519,7 +3905,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -3527,7 +3913,7 @@
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -3551,7 +3937,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23">
         <v>35</v>
@@ -3567,7 +3953,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B25">
         <v>55</v>
@@ -3575,7 +3961,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26">
         <v>35</v>
@@ -3583,7 +3969,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B27">
         <v>35</v>
@@ -3591,7 +3977,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28">
         <v>40</v>
@@ -3599,7 +3985,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29">
         <v>40</v>
@@ -3607,7 +3993,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -3615,7 +4001,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B31">
         <v>45</v>
@@ -3631,7 +4017,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B33">
         <v>22</v>
@@ -3647,7 +4033,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35">
         <v>30</v>
@@ -3655,7 +4041,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36">
         <v>28</v>
@@ -3663,7 +4049,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B37">
         <v>30</v>
@@ -3671,7 +4057,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B38">
         <v>30</v>
@@ -3679,7 +4065,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B39">
         <v>25</v>
@@ -3687,7 +4073,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B40">
         <v>30</v>
@@ -3707,8 +4093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5CF38E-1757-4D28-AE1C-6EFE4AED49B6}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3719,19 +4105,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
         <v>261</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
-      </c>
-      <c r="E1" t="s">
-        <v>263</v>
       </c>
       <c r="F1" t="s">
         <v>271</v>
@@ -3747,7 +4133,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3">
         <v>39</v>
@@ -3755,7 +4141,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4">
         <v>39</v>
@@ -3787,7 +4173,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8">
         <v>47</v>
@@ -3795,7 +4181,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>48</v>
@@ -3859,7 +4245,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17">
         <v>60</v>
@@ -3963,7 +4349,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B30">
         <v>55</v>
@@ -3971,7 +4357,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B31">
         <v>55</v>
@@ -3979,7 +4365,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B32">
         <v>55</v>
@@ -3987,7 +4373,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B33">
         <v>55</v>
@@ -3995,7 +4381,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B34">
         <v>55</v>
@@ -4003,7 +4389,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B35">
         <v>55</v>
@@ -4011,7 +4397,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B36">
         <v>62</v>
@@ -4019,7 +4405,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B37">
         <v>62</v>
@@ -4027,7 +4413,7 @@
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38">
         <v>62</v>
@@ -4035,7 +4421,7 @@
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39">
         <v>62</v>
@@ -4043,7 +4429,7 @@
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40">
         <v>62</v>
@@ -4051,7 +4437,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B41">
         <v>62</v>
@@ -4059,7 +4445,7 @@
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42">
         <v>62</v>
@@ -4067,7 +4453,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -4075,7 +4461,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B44">
         <v>52</v>
@@ -4083,7 +4469,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45">
         <v>46</v>
@@ -4091,7 +4477,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B46">
         <v>46</v>
@@ -4099,7 +4485,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B47">
         <v>56</v>
@@ -4107,7 +4493,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B48">
         <v>56</v>
@@ -4115,7 +4501,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B49">
         <v>56</v>
@@ -4123,7 +4509,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50">
         <v>55</v>
@@ -4131,7 +4517,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B51">
         <v>55</v>
@@ -4139,7 +4525,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B52">
         <v>55</v>
@@ -4155,7 +4541,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B54">
         <v>55</v>
@@ -4163,7 +4549,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55">
         <v>55</v>
@@ -4171,7 +4557,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B56">
         <v>62</v>
@@ -4179,7 +4565,7 @@
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B57">
         <v>62</v>
@@ -4187,7 +4573,7 @@
     </row>
     <row r="58" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B58">
         <v>62</v>
@@ -4195,7 +4581,7 @@
     </row>
     <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B59">
         <v>62</v>
@@ -4203,7 +4589,7 @@
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B60">
         <v>62</v>
@@ -4211,7 +4597,7 @@
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B61">
         <v>62</v>
@@ -4219,7 +4605,7 @@
     </row>
     <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B62">
         <v>62</v>
@@ -4227,7 +4613,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B63">
         <v>42</v>
@@ -4235,7 +4621,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B64">
         <v>52</v>
@@ -4243,7 +4629,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B65">
         <v>46</v>
@@ -4251,7 +4637,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B66">
         <v>46</v>
@@ -4259,7 +4645,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B67">
         <v>56</v>
@@ -4267,7 +4653,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B68">
         <v>56</v>
@@ -4275,7 +4661,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B69">
         <v>56</v>
@@ -4291,6 +4677,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005468605E04F61747936F12076C15E824" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ad5602634390927fddd3c2a70f7b49c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d86c30-c586-4855-827a-97f18e7b00d3" xmlns:ns4="db3c7e19-2d34-4eb7-903f-b25b7c5160ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efd1d29f83cac9fbca6e4254de116c19" ns3:_="" ns4:_="">
     <xsd:import namespace="77d86c30-c586-4855-827a-97f18e7b00d3"/>
@@ -4519,38 +4922,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="77d86c30-c586-4855-827a-97f18e7b00d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
-    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4573,9 +4948,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A22EB8-0E70-4470-8820-36FB34111CB1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB17067-F9E1-4205-8090-57CBC9145BC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="77d86c30-c586-4855-827a-97f18e7b00d3"/>
+    <ds:schemaRef ds:uri="db3c7e19-2d34-4eb7-903f-b25b7c5160ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
El proyecto esta listo
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/menus.xlsx
+++ b/src/main/resources/Data/menus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nintech\Proyectos\Programas\java\WherEat\WherEat\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3538C9C-FA07-4A4C-AF18-3F63D2FD8BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF248075-BBFC-42F5-B5D3-915653870B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20460" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{B861746F-D976-495D-8CE6-BDF99A1F637C}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="284">
   <si>
     <t>Precio</t>
   </si>
@@ -816,15 +816,6 @@
     <t>Aram</t>
   </si>
   <si>
-    <t>Gonzales</t>
-  </si>
-  <si>
-    <t>correogenerico@gmail.com</t>
-  </si>
-  <si>
-    <t>algo1234</t>
-  </si>
-  <si>
     <t>contraseña</t>
   </si>
   <si>
@@ -864,49 +855,49 @@
     <t>Economia</t>
   </si>
   <si>
+    <t xml:space="preserve">Facultad de Ingenieria Edificio G </t>
+  </si>
+  <si>
+    <t>Puesto de Comida</t>
+  </si>
+  <si>
+    <t>Café</t>
+  </si>
+  <si>
+    <t>Enchiladas</t>
+  </si>
+  <si>
+    <t>Café Cappuchino Largo</t>
+  </si>
+  <si>
+    <t>Café Cappuchino Corto</t>
+  </si>
+  <si>
+    <t>Chapata Italiana</t>
+  </si>
+  <si>
+    <t>Chapata Tropical</t>
+  </si>
+  <si>
+    <t>Facultad de Arquitectura - Café</t>
+  </si>
+  <si>
     <t>Juan Carlos</t>
   </si>
   <si>
     <t>Bodoque</t>
   </si>
   <si>
-    <t>juan@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facultad de Ingenieria Edificio G </t>
-  </si>
-  <si>
-    <t>Puesto de Comida</t>
-  </si>
-  <si>
-    <t>Café</t>
-  </si>
-  <si>
-    <t>Enchiladas</t>
-  </si>
-  <si>
-    <t>Café Cappuchino Largo</t>
-  </si>
-  <si>
-    <t>Café Cappuchino Corto</t>
-  </si>
-  <si>
-    <t>Chapata Italiana</t>
-  </si>
-  <si>
-    <t>Chapata Tropical</t>
-  </si>
-  <si>
-    <t>Facultad de Arquitectura - Café</t>
-  </si>
-  <si>
-    <t>Alguna</t>
-  </si>
-  <si>
-    <t>Persona</t>
-  </si>
-  <si>
-    <t>persona@gmail.com</t>
+    <t>juancarlos@gmail.com</t>
+  </si>
+  <si>
+    <t>Gonzales Ronquillo</t>
+  </si>
+  <si>
+    <t>araamglezr@gmail.com</t>
+  </si>
+  <si>
+    <t>A12345678</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1034,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <border outline="0">
         <bottom style="thick">
@@ -1164,6 +1155,9 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1184,7 +1178,7 @@
     <tableColumn id="1" xr3:uid="{04D57AF8-9FFB-4E94-AF07-AFAC6C77B6D3}" name="Nombres"/>
     <tableColumn id="2" xr3:uid="{716EEDB6-DE4B-45B8-8104-3D089AF9A671}" name="Apellidos"/>
     <tableColumn id="3" xr3:uid="{4126AD90-CEFD-435C-8233-2C25FE9525E8}" name="Correo" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="4" xr3:uid="{6BDCA459-9465-4048-B42D-264D76C79C9D}" name="Contraseña"/>
+    <tableColumn id="4" xr3:uid="{6BDCA459-9465-4048-B42D-264D76C79C9D}" name="Contraseña" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1637,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECF5DA-6B46-4C56-8004-333EE01336D6}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1669,7 @@
       <c r="C2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>251</v>
       </c>
     </row>
@@ -1689,8 +1683,8 @@
       <c r="C3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D3" t="s">
-        <v>259</v>
+      <c r="D3" s="5" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,55 +1692,39 @@
         <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D4" t="s">
-        <v>258</v>
+        <v>281</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="4"/>
+        <v>280</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>256</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F099B287-23BF-45F2-A67E-A80C884E73AA}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{2FB42FF3-BBE0-44FB-81EC-DD3540E13B5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1767,27 +1745,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B2">
         <v>35</v>
@@ -1795,7 +1773,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B3">
         <v>28</v>
@@ -1803,7 +1781,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1811,7 +1789,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -1840,27 +1818,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B2">
         <v>35</v>
@@ -1868,7 +1846,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B3">
         <v>28</v>
@@ -1876,7 +1854,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B4">
         <v>30</v>
@@ -1884,7 +1862,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -1923,16 +1901,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" t="s">
         <v>260</v>
-      </c>
-      <c r="D1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2257,7 +2235,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -2325,16 +2303,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" t="s">
         <v>261</v>
-      </c>
-      <c r="E1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2559,16 +2537,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F1" t="s">
         <v>262</v>
-      </c>
-      <c r="F1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2786,16 +2764,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3151,22 +3129,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3528,16 +3506,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3755,16 +3733,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4111,16 +4089,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>